<commit_message>
Updated config calls within intialization and exit, pulled moving the email into it's own workflow
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\RpaUiPathProcess\Processes\RPATask1-ChartStringProformaDetail\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -55,42 +55,8 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Samuel Janetzki</author>
-  </authors>
-  <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Samuel Janetzki:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-(separate Name and Envirment with "-")</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="156">
   <si>
     <t>Name</t>
   </si>
@@ -101,599 +67,470 @@
     <t>Asset</t>
   </si>
   <si>
+    <t>TimeoutShort</t>
+  </si>
+  <si>
+    <t>Timeout short value in milliseconds, for activities which are likely to fail. Must be integer</t>
+  </si>
+  <si>
+    <t>TimeoutMedium</t>
+  </si>
+  <si>
+    <t>Timeout medium value in milliseconds. Must be integer</t>
+  </si>
+  <si>
+    <t>TimeoutLong</t>
+  </si>
+  <si>
+    <t>Timeout short value in milliseconds, for slow apps. Must be integer</t>
+  </si>
+  <si>
+    <t>ExScreenshotsFolderPath</t>
+  </si>
+  <si>
+    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
+  </si>
+  <si>
+    <t>DelayShort</t>
+  </si>
+  <si>
+    <t>Delay short value in milliseconds, for activities where it is necessary to wait a little. Must be integer</t>
+  </si>
+  <si>
+    <t>DelayMedium</t>
+  </si>
+  <si>
+    <t>Delay medium value in milliseconds, for activities where it is necessary to wait a moderate amount of time. Must be integer</t>
+  </si>
+  <si>
+    <t>DelayLong</t>
+  </si>
+  <si>
+    <t>Delay long value in milliseconds, for activities where it is necessary to wait a long time. Must be integer</t>
+  </si>
+  <si>
+    <t>AccuracyLow</t>
+  </si>
+  <si>
+    <t>Image accuracy low value, for images that have high contrast. Must be double</t>
+  </si>
+  <si>
+    <t>AccuracyMedium</t>
+  </si>
+  <si>
+    <t>Image accuracy medium value, for images that have normal contrast. Must be double</t>
+  </si>
+  <si>
+    <t>AccuracyHigh</t>
+  </si>
+  <si>
+    <t>Image accuracy high value, for images that have low contrast. Must be double</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionData</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Processing Transaction Number: </t>
+  </si>
+  <si>
+    <t>Static part of logging message. Calling Get Transaction Data</t>
+  </si>
+  <si>
+    <t>LogMessage_GetTransactionDataError</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Error retrieving Transaction Data.</t>
+  </si>
+  <si>
+    <t>LogMessage_Success</t>
+  </si>
+  <si>
+    <t>Transaction Successful.</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction succesful</t>
+  </si>
+  <si>
+    <t>LogMessage_ApplicationException</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction failed with application exception</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
+  </si>
+  <si>
+    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
+  </si>
+  <si>
+    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>Grants\Proposals\Maintain Staged Proposals</t>
+  </si>
+  <si>
+    <t>Path from main menu to Proforma entry</t>
+  </si>
+  <si>
+    <t>System Error</t>
+  </si>
+  <si>
+    <t>4.2</t>
+  </si>
+  <si>
+    <t>Invalid Proforma Data</t>
+  </si>
+  <si>
+    <t>7.1</t>
+  </si>
+  <si>
+    <t>7.2-6</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>8.2</t>
+  </si>
+  <si>
+    <t>Accountant Not Found</t>
+  </si>
+  <si>
+    <t>9.1-5</t>
+  </si>
+  <si>
+    <t>I couldn't match {0} to an accountant name</t>
+  </si>
+  <si>
+    <t>SystemError_InitExchange</t>
+  </si>
+  <si>
+    <t>SystemError_AccountantFile</t>
+  </si>
+  <si>
+    <t>SystemError_LoginUniFi</t>
+  </si>
+  <si>
+    <t>SystemError_NavigateUniFi</t>
+  </si>
+  <si>
+    <t>RuleException_ValidateProforma</t>
+  </si>
+  <si>
+    <t>RuleException_ValidateRMNum</t>
+  </si>
+  <si>
+    <t>RuleException_SearchRMNum</t>
+  </si>
+  <si>
+    <t>10.1</t>
+  </si>
+  <si>
+    <t>Exchange Error</t>
+  </si>
+  <si>
+    <t>Network Error</t>
+  </si>
+  <si>
+    <t>9.7-10</t>
+  </si>
+  <si>
+    <t>Invalid RM Number</t>
+  </si>
+  <si>
+    <t>No Search Results</t>
+  </si>
+  <si>
+    <t>No Updated Entries</t>
+  </si>
+  <si>
+    <t>SystemError_ProformaEntry</t>
+  </si>
+  <si>
+    <t>10.2-11.3</t>
+  </si>
+  <si>
+    <t>12.1-9</t>
+  </si>
+  <si>
+    <t>I searched for {0} and found no results</t>
+  </si>
+  <si>
+    <t>RuleException_NoEmails</t>
+  </si>
+  <si>
+    <t>No Emails Found</t>
+  </si>
+  <si>
+    <t>14.1</t>
+  </si>
+  <si>
+    <t>I couldn't create the folder at {0}</t>
+  </si>
+  <si>
+    <t>14.2</t>
+  </si>
+  <si>
+    <t>SystemError_CreateFolder</t>
+  </si>
+  <si>
+    <t>SystemError_SaveEmail</t>
+  </si>
+  <si>
+    <t>I couldn't save the email to {0}</t>
+  </si>
+  <si>
+    <t>UniFiPath_MaintainStagedProposals</t>
+  </si>
+  <si>
+    <t>SystemError_CheckExchange</t>
+  </si>
+  <si>
+    <t>UniFi Login Error</t>
+  </si>
+  <si>
+    <t>UniFi Navigation Error</t>
+  </si>
+  <si>
+    <t>UniFi Updating Error</t>
+  </si>
+  <si>
+    <t>RuleException_SearchAccountant</t>
+  </si>
+  <si>
+    <t>I got lost while navigating to {0}</t>
+  </si>
+  <si>
+    <t>SystemError_UnhandledUniFi</t>
+  </si>
+  <si>
+    <t>9.1-12.9</t>
+  </si>
+  <si>
+    <t>UniFi Unknown Error</t>
+  </si>
+  <si>
+    <t>I wasn't able to update {0} as the rows were: {1}</t>
+  </si>
+  <si>
+    <t>RuleException_UpdateProforma</t>
+  </si>
+  <si>
+    <t>I couldn't update row {0} due to: {1}</t>
+  </si>
+  <si>
+    <t>SystemError_UnhandledExchange</t>
+  </si>
+  <si>
+    <t>7.1-6</t>
+  </si>
+  <si>
+    <t>Unknown Scrape Error</t>
+  </si>
+  <si>
+    <t>I couldn't scrape proforma data from the email {0}</t>
+  </si>
+  <si>
+    <t>LogMessage_SkippedProforma</t>
+  </si>
+  <si>
+    <t>LogMessage_UpdatedProforma</t>
+  </si>
+  <si>
+    <t>Row {0} skipped, {1}</t>
+  </si>
+  <si>
+    <t>Row {0} updated, {1}</t>
+  </si>
+  <si>
+    <t>Problems loading {0} for Acc lookup: {1} at: {2}</t>
+  </si>
+  <si>
+    <t>Problems with {0}'s mail: {1} at: {2}</t>
+  </si>
+  <si>
+    <t>Problems checking {0} as {1}: {2} at {3}</t>
+  </si>
+  <si>
+    <t>Login issue as {0} to UniFi at {1}: {2} at {3}</t>
+  </si>
+  <si>
+    <t>ExchangeExitErrors</t>
+  </si>
+  <si>
+    <t>ExchangeExitSuccess</t>
+  </si>
+  <si>
+    <t>Proforma documents processed successfully</t>
+  </si>
+  <si>
+    <t>Errors processing proforma documents</t>
+  </si>
+  <si>
+    <t>Minion</t>
+  </si>
+  <si>
+    <t>ChartStringProforma</t>
+  </si>
+  <si>
+    <t>SystemError_FileServer</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>File Server Access</t>
+  </si>
+  <si>
+    <t>Mode Asset Missing</t>
+  </si>
+  <si>
+    <t>I couldn't map {0} due to: {1}</t>
+  </si>
+  <si>
+    <t>Config Not Initialised</t>
+  </si>
+  <si>
+    <t>I couldn't get my settings from the config: {0}</t>
+  </si>
+  <si>
+    <t>https://outlook.office365.com/EWS/Exchange.asmx</t>
+  </si>
+  <si>
+    <t>I couldn't find my operation mode asset at OperatingEnvironment</t>
+  </si>
+  <si>
+    <t>Exceptions_Screenshots</t>
+  </si>
+  <si>
+    <t>SSO_rpa00002</t>
+  </si>
+  <si>
+    <t>I couldn't validate {0} in the proforma email</t>
+  </si>
+  <si>
+    <t>The RM number is missing or the email is not a proforma template</t>
+  </si>
+  <si>
+    <t>I couldn't find any emails in {0}</t>
+  </si>
+  <si>
+    <t>ProcessName</t>
+  </si>
+  <si>
+    <t>TransactionItem</t>
+  </si>
+  <si>
+    <t>proforma email</t>
+  </si>
+  <si>
+    <t>The descriptive name of the transaction items for human readability</t>
+  </si>
+  <si>
+    <t>Sheet1</t>
+  </si>
+  <si>
+    <t>UniFi_URL</t>
+  </si>
+  <si>
+    <t>NetworkShare_DownloadFolder</t>
+  </si>
+  <si>
+    <t>Credentials_UniFi</t>
+  </si>
+  <si>
+    <t>Credentials_FileServing</t>
+  </si>
+  <si>
+    <t>Credentials_Tester</t>
+  </si>
+  <si>
+    <t>Proforma_UniFi_Tester</t>
+  </si>
+  <si>
+    <t>Proforma_UniFi_URL</t>
+  </si>
+  <si>
+    <t>Proforma_FileShare_SaveFolder</t>
+  </si>
+  <si>
+    <t>Proforma_FileShare_AccountantUsernameLookup</t>
+  </si>
+  <si>
+    <t>Accountant_LookupWorkbook</t>
+  </si>
+  <si>
+    <t>Credentials_Exchange</t>
+  </si>
+  <si>
+    <t>Accountant_LookupSheet</t>
+  </si>
+  <si>
+    <t>Exchange_ServerName</t>
+  </si>
+  <si>
+    <t>JobReport_Recipients</t>
+  </si>
+  <si>
+    <t>SystemError_NotificationEmail</t>
+  </si>
+  <si>
+    <t>SystemError_Recipients</t>
+  </si>
+  <si>
+    <t>ExchangeInbox</t>
+  </si>
+  <si>
+    <t>ExchangeOutbox</t>
+  </si>
+  <si>
+    <t>ExchangeExceptions</t>
+  </si>
+  <si>
+    <t>Extras</t>
+  </si>
+  <si>
     <t>Description</t>
   </si>
   <si>
-    <t>TimeoutShort</t>
-  </si>
-  <si>
-    <t>Timeout short value in milliseconds, for activities which are likely to fail. Must be integer</t>
-  </si>
-  <si>
-    <t>TimeoutMedium</t>
-  </si>
-  <si>
-    <t>Timeout medium value in milliseconds. Must be integer</t>
-  </si>
-  <si>
-    <t>TimeoutLong</t>
-  </si>
-  <si>
-    <t>Timeout short value in milliseconds, for slow apps. Must be integer</t>
-  </si>
-  <si>
-    <t>ExScreenshotsFolderPath</t>
-  </si>
-  <si>
-    <t>Where to save exceptions screenshots - can be a full or a relative path.</t>
-  </si>
-  <si>
-    <t>DelayShort</t>
-  </si>
-  <si>
-    <t>Delay short value in milliseconds, for activities where it is necessary to wait a little. Must be integer</t>
-  </si>
-  <si>
-    <t>DelayMedium</t>
-  </si>
-  <si>
-    <t>Delay medium value in milliseconds, for activities where it is necessary to wait a moderate amount of time. Must be integer</t>
-  </si>
-  <si>
-    <t>DelayLong</t>
-  </si>
-  <si>
-    <t>Delay long value in milliseconds, for activities where it is necessary to wait a long time. Must be integer</t>
-  </si>
-  <si>
-    <t>AccuracyLow</t>
-  </si>
-  <si>
-    <t>Image accuracy low value, for images that have high contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyMedium</t>
-  </si>
-  <si>
-    <t>Image accuracy medium value, for images that have normal contrast. Must be double</t>
-  </si>
-  <si>
-    <t>AccuracyHigh</t>
-  </si>
-  <si>
-    <t>Image accuracy high value, for images that have low contrast. Must be double</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionData</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
-    <t>Static part of logging message. Calling Get Transaction Data</t>
-  </si>
-  <si>
-    <t>LogMessage_GetTransactionDataError</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Error retrieving Transaction Data.</t>
-  </si>
-  <si>
-    <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction succesful</t>
-  </si>
-  <si>
-    <t>LogMessage_ApplicationException</t>
-  </si>
-  <si>
-    <t>Static part of logging message. Processed Transaction failed with application exception</t>
-  </si>
-  <si>
-    <t>OrchestratorQueueName</t>
-  </si>
-  <si>
-    <t>Orchestrator Queue Name. Be sure to match this name with the one from the server.</t>
-  </si>
-  <si>
-    <t>This is a logging field which allows you to group the log data of two or more subprocesses under the same business process name</t>
-  </si>
-  <si>
-    <t>Credential</t>
-  </si>
-  <si>
-    <t>Development\Proforma\Robot Out</t>
-  </si>
-  <si>
-    <t>Development\Proforma\Robot Error</t>
-  </si>
-  <si>
-    <t>Development\Proforma\Robot In</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>https://fs92rept.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
-  </si>
-  <si>
-    <t>5.1</t>
-  </si>
-  <si>
-    <t>Grants\Proposals\Maintain Staged Proposals</t>
-  </si>
-  <si>
-    <t>Path from main menu to Proforma entry</t>
-  </si>
-  <si>
-    <t>System Error</t>
-  </si>
-  <si>
-    <t>4.2</t>
-  </si>
-  <si>
-    <t>Invalid Proforma Data</t>
-  </si>
-  <si>
-    <t>7.1</t>
-  </si>
-  <si>
-    <t>7.2-6</t>
-  </si>
-  <si>
-    <t>8.1</t>
-  </si>
-  <si>
-    <t>8.2</t>
-  </si>
-  <si>
-    <t>Accountant Not Found</t>
-  </si>
-  <si>
-    <t>9.1-5</t>
-  </si>
-  <si>
-    <t>I couldn't match {0} to an accountant name</t>
-  </si>
-  <si>
-    <t>SystemError_InitExchange</t>
-  </si>
-  <si>
-    <t>SystemError_AccountantFile</t>
-  </si>
-  <si>
-    <t>SystemError_LoginUniFi</t>
-  </si>
-  <si>
-    <t>SystemError_NavigateUniFi</t>
-  </si>
-  <si>
-    <t>RuleException_ValidateProforma</t>
-  </si>
-  <si>
-    <t>RuleException_ValidateRMNum</t>
-  </si>
-  <si>
-    <t>RuleException_SearchRMNum</t>
-  </si>
-  <si>
-    <t>10.1</t>
-  </si>
-  <si>
-    <t>Exchange Error</t>
-  </si>
-  <si>
-    <t>Network Error</t>
-  </si>
-  <si>
-    <t>9.7-10</t>
-  </si>
-  <si>
-    <t>Invalid RM Number</t>
-  </si>
-  <si>
-    <t>No Search Results</t>
-  </si>
-  <si>
-    <t>No Updated Entries</t>
-  </si>
-  <si>
-    <t>SystemError_ProformaEntry</t>
-  </si>
-  <si>
-    <t>10.2-11.3</t>
-  </si>
-  <si>
-    <t>12.1-9</t>
-  </si>
-  <si>
-    <t>I searched for {0} and found no results</t>
-  </si>
-  <si>
-    <t>RuleException_NoEmails</t>
-  </si>
-  <si>
-    <t>No Emails Found</t>
-  </si>
-  <si>
-    <t>14.1</t>
-  </si>
-  <si>
-    <t>I couldn't create the folder at {0}</t>
-  </si>
-  <si>
-    <t>14.2</t>
-  </si>
-  <si>
-    <t>SystemError_CreateFolder</t>
-  </si>
-  <si>
-    <t>SystemError_SaveEmail</t>
-  </si>
-  <si>
-    <t>I couldn't save the email to {0}</t>
-  </si>
-  <si>
-    <t>UniFiPath_MaintainStagedProposals</t>
-  </si>
-  <si>
-    <t>SystemError_CheckExchange</t>
-  </si>
-  <si>
-    <t>UniFi Login Error</t>
-  </si>
-  <si>
-    <t>UniFi Navigation Error</t>
-  </si>
-  <si>
-    <t>UniFi Updating Error</t>
-  </si>
-  <si>
-    <t>RuleException_SearchAccountant</t>
-  </si>
-  <si>
-    <t>I got lost while navigating to {0}</t>
-  </si>
-  <si>
-    <t>SystemError_UnhandledUniFi</t>
-  </si>
-  <si>
-    <t>9.1-12.9</t>
-  </si>
-  <si>
-    <t>UniFi Unknown Error</t>
-  </si>
-  <si>
-    <t>I wasn't able to update {0} as the rows were: {1}</t>
-  </si>
-  <si>
-    <t>RuleException_UpdateProforma</t>
-  </si>
-  <si>
-    <t>I couldn't update row {0} due to: {1}</t>
-  </si>
-  <si>
-    <t>SystemError_UnhandledExchange</t>
-  </si>
-  <si>
-    <t>7.1-6</t>
-  </si>
-  <si>
-    <t>Unknown Scrape Error</t>
-  </si>
-  <si>
-    <t>I couldn't scrape proforma data from the email {0}</t>
-  </si>
-  <si>
-    <t>LogMessage_SkippedProforma</t>
-  </si>
-  <si>
-    <t>LogMessage_UpdatedProforma</t>
-  </si>
-  <si>
-    <t>Row {0} skipped, {1}</t>
-  </si>
-  <si>
-    <t>Row {0} updated, {1}</t>
-  </si>
-  <si>
-    <t>Minion logo for email signature</t>
-  </si>
-  <si>
-    <t>HTML file containing parts to build end of job report</t>
-  </si>
-  <si>
-    <t>Accountant username lookup file</t>
-  </si>
-  <si>
-    <t>Nvision</t>
-  </si>
-  <si>
-    <t>Problems loading {0} for Acc lookup: {1} at: {2}</t>
-  </si>
-  <si>
-    <t>Problems with {0}'s mail: {1} at: {2}</t>
-  </si>
-  <si>
-    <t>Problems checking {0} as {1}: {2} at {3}</t>
-  </si>
-  <si>
-    <t>Login issue as {0} to UniFi at {1}: {2} at {3}</t>
-  </si>
-  <si>
-    <t>ExchangeExitErrors</t>
-  </si>
-  <si>
-    <t>ExchangeExitSuccess</t>
-  </si>
-  <si>
-    <t>Proforma documents processed successfully</t>
-  </si>
-  <si>
-    <t>Errors processing proforma documents</t>
-  </si>
-  <si>
-    <t>Comments</t>
-  </si>
-  <si>
-    <t>Comments (Assets will always overwrite other config)</t>
-  </si>
-  <si>
-    <t>Minion</t>
-  </si>
-  <si>
-    <t>Testing_ReportWorkbook</t>
-  </si>
-  <si>
-    <t>Location of the test file to output results of job report generation</t>
-  </si>
-  <si>
-    <t>Testing_ReportSheet</t>
-  </si>
-  <si>
-    <t>Worksheet to output results of test job report generation</t>
-  </si>
-  <si>
-    <t>Testing_SummaryWorkbook</t>
-  </si>
-  <si>
-    <t>Testing_SummarySheet</t>
-  </si>
-  <si>
-    <t>Worksheet to output results of test weekly summary generation</t>
-  </si>
-  <si>
-    <t>Location of the test file to output results of weekly summary generation</t>
-  </si>
-  <si>
-    <t>ChartStringProforma</t>
-  </si>
-  <si>
-    <t>SSO_RPA_Sam</t>
-  </si>
-  <si>
-    <t>SystemError_FileServer</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>File Server Access</t>
-  </si>
-  <si>
-    <t>Mode Asset Missing</t>
-  </si>
-  <si>
-    <t>I couldn't map {0} due to: {1}</t>
-  </si>
-  <si>
-    <t>Config Not Initialised</t>
-  </si>
-  <si>
-    <t>I couldn't get my settings from the config: {0}</t>
-  </si>
-  <si>
-    <t>https://outlook.office365.com/EWS/Exchange.asmx</t>
-  </si>
-  <si>
-    <t>Proforma-DEV-UniFi</t>
-  </si>
-  <si>
-    <t>\\nas02.storage.uq.edu.au\CA\FBS\test\Accountant Lookup.xlsx</t>
-  </si>
-  <si>
-    <t>I couldn't find my operation mode asset at OperatingEnvironment</t>
-  </si>
-  <si>
-    <t>Exceptions_Screenshots</t>
-  </si>
-  <si>
-    <t>Credentials_UniFi-DEV</t>
-  </si>
-  <si>
-    <t>Credentials_FileServing-DEV</t>
-  </si>
-  <si>
-    <t>Credentials_Exchange-DEV</t>
-  </si>
-  <si>
-    <t>SSO_rpa00002</t>
-  </si>
-  <si>
-    <t>Credentials_UniFi-UAT_STG_PRD</t>
-  </si>
-  <si>
-    <t>Credentials_FileServing-UAT_STG_PRD</t>
-  </si>
-  <si>
-    <t>Credentials_Exchange-UAT_STG_PRD</t>
-  </si>
-  <si>
-    <t>https://www.unifi.uq.edu.au/psp/ps/?cmd=login</t>
-  </si>
-  <si>
-    <t>\\nas02.storage.uq.edu.au\CA\FBS\test\{0}\</t>
-  </si>
-  <si>
-    <t>NetworkShare_DownloadFolder-DEV</t>
-  </si>
-  <si>
-    <t>NetworkShare_DownloadFolder-PRD</t>
-  </si>
-  <si>
-    <t>NetworkShare_DownloadFolder-UAT_STG</t>
-  </si>
-  <si>
-    <t>Exchange_ServerName-DEV_UAT_STG_PRD</t>
-  </si>
-  <si>
-    <t>Accountant_LookupWorkbook-DEV</t>
-  </si>
-  <si>
-    <t>ExchangeInbox-DEV</t>
-  </si>
-  <si>
-    <t>ExchangeInbox-UAT_STG</t>
-  </si>
-  <si>
-    <t>ExchangeInbox-PRD</t>
-  </si>
-  <si>
-    <t>ExchangeOutbox-DEV</t>
-  </si>
-  <si>
-    <t>ExchangeOutbox-UAT_STG</t>
-  </si>
-  <si>
-    <t>ExchangeExceptions-DEV</t>
-  </si>
-  <si>
-    <t>ExchangeExceptions-UAT_STG</t>
-  </si>
-  <si>
-    <t>ExchangeExceptions-PRD</t>
-  </si>
-  <si>
-    <t>I couldn't validate {0} in the proforma email</t>
-  </si>
-  <si>
-    <t>The RM number is missing or the email is not a proforma template</t>
-  </si>
-  <si>
-    <t>I couldn't find any emails in {0}</t>
-  </si>
-  <si>
-    <t>ProcessName</t>
-  </si>
-  <si>
-    <t>HtmlLogo</t>
-  </si>
-  <si>
-    <t>HtmlTemplate</t>
-  </si>
-  <si>
-    <t>TransactionItem</t>
-  </si>
-  <si>
-    <t>proforma email</t>
-  </si>
-  <si>
-    <t>The descriptive name of the transaction items for human readability</t>
-  </si>
-  <si>
-    <t>Data\report.html</t>
-  </si>
-  <si>
-    <t>Data\logo.png</t>
-  </si>
-  <si>
-    <t>Proforma-DEV-EmailRecipients</t>
-  </si>
-  <si>
-    <t>JobReport_Recipients-DEV</t>
-  </si>
-  <si>
-    <t>JobReport_Recipients-PRD</t>
-  </si>
-  <si>
-    <t>JobReport_Recipients-UAT</t>
-  </si>
-  <si>
-    <t>JobReport_Recipients-STG</t>
-  </si>
-  <si>
-    <t>Proforma-UAT-EmailRecipients</t>
-  </si>
-  <si>
-    <t>Proforma-STG-EmailRecipients</t>
-  </si>
-  <si>
-    <t>Proforma-PRD-EmailRecipients</t>
-  </si>
-  <si>
-    <t>\\nas02.storage.uq.edu.au\CA\FBS\Contract and Grants Accounting\General\GRLS\No project GRLS\{0}\</t>
-  </si>
-  <si>
-    <t>\\nas02.storage.uq.edu.au\CA\FBS\Contract and Grants Accounting\General\GRLS\Accountant Lookup.xlsx</t>
-  </si>
-  <si>
-    <t>Sheet1</t>
-  </si>
-  <si>
-    <t>Accountant_LookupSheet-DEV_UAT</t>
-  </si>
-  <si>
-    <t>Accountant_LookupSheet-STG_PRD</t>
-  </si>
-  <si>
-    <t>Accountant_LookupWorkbook-UAT</t>
-  </si>
-  <si>
-    <t>Accountant_LookupWorkbook-STG_PRD</t>
-  </si>
-  <si>
-    <t>contractandgrants@uq.edu.au\Inbox\Minion\Testing\New</t>
-  </si>
-  <si>
-    <t>contractandgrants@uq.edu.au\Inbox\Minion\New</t>
-  </si>
-  <si>
-    <t>contractandgrants@uq.edu.au\Inbox\Minion\Testing</t>
-  </si>
-  <si>
-    <t>contractandgrants@uq.edu.au\Inbox\Minion\Testing\Error</t>
-  </si>
-  <si>
-    <t>contractandgrants@uq.edu.au\Inbox\Minion\Error</t>
-  </si>
-  <si>
-    <t>UniFi_URL-DEV_TEST</t>
-  </si>
-  <si>
-    <t>UniFi_URL-STAGING_PROD</t>
-  </si>
-  <si>
-    <t>s</t>
+    <t>Description (Assets will always overwrite other config)</t>
+  </si>
+  <si>
+    <t>Exchange_Mailbox</t>
+  </si>
+  <si>
+    <t>Proforma_Exchange_RootFolder</t>
+  </si>
+  <si>
+    <t>Proforma_EmailRecipients</t>
+  </si>
+  <si>
+    <t>\New</t>
+  </si>
+  <si>
+    <t>\Error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -725,6 +562,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -746,7 +589,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -757,6 +600,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1036,30 +880,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1012"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68" customWidth="1"/>
-    <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="68.5703125" customWidth="1"/>
+    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="118.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>118</v>
+      <c r="C1" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -1085,98 +929,57 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B4" s="9"/>
+        <v>125</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>151</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="9"/>
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>151</v>
+        <v>128</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>184</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1184,186 +987,91 @@
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>140</v>
+        <v>79</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" t="s">
-        <v>108</v>
-      </c>
+      <c r="A10" s="2"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>185</v>
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>119</v>
       </c>
       <c r="C11" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>188</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>146</v>
+      </c>
       <c r="B14" s="9"/>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B15" s="9" t="s">
-        <v>138</v>
-      </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>40</v>
-      </c>
+      <c r="A16" s="2"/>
+      <c r="B16" s="9"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="B18" s="9" t="s">
-        <v>192</v>
-      </c>
+      <c r="A17" s="2"/>
+      <c r="B17" s="9"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B21" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="9"/>
-    </row>
-    <row r="26" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-    </row>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>121</v>
-      </c>
-      <c r="C46" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>123</v>
-      </c>
-      <c r="C47" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>125</v>
-      </c>
-      <c r="C48" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>126</v>
-      </c>
-      <c r="C49" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="9"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="9"/>
+    </row>
+    <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2306,35 +2014,31 @@
     <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1009" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1010" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1011" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1012" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B11" r:id="rId1" display="\\nas02.storage.uq.edu.au\CA\FBS\test\Exceptions_Screenshots"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA989"/>
+  <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.42578125" customWidth="1"/>
-    <col min="2" max="3" width="15.7109375" customWidth="1"/>
-    <col min="4" max="27" width="65.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="26" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2342,11 +2046,9 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>119</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2369,109 +2071,116 @@
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-    </row>
-    <row r="2" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="B12" t="s">
         <v>143</v>
       </c>
-      <c r="C2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="6" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="7" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C8" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="14" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="15" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>151</v>
+      </c>
+      <c r="B13" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="9"/>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="9"/>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="9"/>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3429,6 +3138,7 @@
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3437,7 +3147,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
@@ -3446,20 +3156,20 @@
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53" customWidth="1"/>
-    <col min="2" max="2" width="63.5703125" customWidth="1"/>
+    <col min="2" max="2" width="41" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="89" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>118</v>
+      <c r="C1" s="10" t="s">
+        <v>149</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3487,205 +3197,140 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>168</v>
-      </c>
-      <c r="B2" t="s">
-        <v>120</v>
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>5000</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>30000</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>171</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>172</v>
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>120000</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>5000</v>
+        <v>1000</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <v>30000</v>
+        <v>15000</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <v>120000</v>
+        <v>60000</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <v>1000</v>
+        <v>0.6</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B11">
-        <v>15000</v>
+        <v>0.8</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="B12">
-        <v>60000</v>
+        <v>0.9</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14">
-        <v>0.6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15">
-        <v>0.8</v>
-      </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="B15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16">
-        <v>0.9</v>
-      </c>
-      <c r="C16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="B16" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="C20" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>115</v>
-      </c>
-      <c r="B23" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="C25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4648,35 +4293,25 @@
     <row r="992" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="993" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="994" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="995" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="1001" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" display="\\nas02.storage.uq.edu.au\CA\FBS\test\Exceptions_Screenshots"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.7109375" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" style="4" customWidth="1"/>
-    <col min="3" max="3" width="63.5703125" customWidth="1"/>
-    <col min="4" max="4" width="60.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.42578125" customWidth="1"/>
+    <col min="4" max="4" width="83.42578125" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4685,54 +4320,54 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>118</v>
+        <v>148</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>141</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4740,301 +4375,293 @@
       <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>167</v>
+        <v>65</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>58</v>
+        <v>45</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>53</v>
+        <v>58</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>79</v>
+        <v>53</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>80</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>50</v>
+        <v>92</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>93</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>50</v>
+        <v>55</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>112</v>
+        <v>81</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>99</v>
+        <v>56</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>57</v>
+        <v>67</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>113</v>
+        <v>83</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="D23" s="2" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>75</v>
+        <v>86</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>84</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="D24" s="5"/>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B26" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D26" s="5"/>
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" t="s">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C28" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="D29" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>24</v>
-      </c>
-      <c r="C30" t="s">
-        <v>25</v>
-      </c>
-      <c r="D30" t="s">
-        <v>26</v>
+        <v>96</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" t="s">
-        <v>30</v>
-      </c>
-      <c r="D31" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>103</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated asset names in orch, dev tests verified and ready for test env
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="154">
   <si>
     <t>Name</t>
   </si>
@@ -418,9 +418,6 @@
     <t>Exceptions_Screenshots</t>
   </si>
   <si>
-    <t>SSO_rpa00002</t>
-  </si>
-  <si>
     <t>I couldn't validate {0} in the proforma email</t>
   </si>
   <si>
@@ -457,21 +454,6 @@
     <t>Credentials_FileServing</t>
   </si>
   <si>
-    <t>Credentials_Tester</t>
-  </si>
-  <si>
-    <t>Proforma_UniFi_Tester</t>
-  </si>
-  <si>
-    <t>Proforma_UniFi_URL</t>
-  </si>
-  <si>
-    <t>Proforma_FileShare_SaveFolder</t>
-  </si>
-  <si>
-    <t>Proforma_FileShare_AccountantUsernameLookup</t>
-  </si>
-  <si>
     <t>Accountant_LookupWorkbook</t>
   </si>
   <si>
@@ -514,16 +496,28 @@
     <t>Exchange_Mailbox</t>
   </si>
   <si>
-    <t>Proforma_Exchange_RootFolder</t>
-  </si>
-  <si>
-    <t>Proforma_EmailRecipients</t>
-  </si>
-  <si>
     <t>\New</t>
   </si>
   <si>
     <t>\Error</t>
+  </si>
+  <si>
+    <t>FA_Proforma_Exchange_RootFolder</t>
+  </si>
+  <si>
+    <t>FA_Proforma_FileShare_AccountantLookup</t>
+  </si>
+  <si>
+    <t>FA_Proforma_FileShare_SaveFolder</t>
+  </si>
+  <si>
+    <t>FA_Proforma_ReportRecipients</t>
+  </si>
+  <si>
+    <t>FA_Proforma_SSO_rpa00002</t>
+  </si>
+  <si>
+    <t>FA_Proforma_UniFi_URL</t>
   </si>
 </sst>
 </file>
@@ -883,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -903,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -931,7 +925,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
         <v>108</v>
@@ -953,13 +947,13 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" t="s">
         <v>126</v>
-      </c>
-      <c r="C4" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -968,15 +962,15 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>117</v>
@@ -1012,24 +1006,24 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B14" s="9"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -2025,10 +2019,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z990"/>
+  <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2040,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2074,99 +2068,92 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B5" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>120</v>
+      <c r="B6" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B8" t="s">
-        <v>137</v>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>120</v>
+        <v>136</v>
+      </c>
+      <c r="B10" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="B13" t="s">
-        <v>152</v>
-      </c>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="9"/>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="9"/>
     </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="9"/>
-    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="9"/>
-    </row>
+    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="9"/>
+    </row>
+    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3138,7 +3125,6 @@
     <row r="987" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="988" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="989" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="990" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3169,7 +3155,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4326,10 +4312,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4385,7 +4371,7 @@
         <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4427,7 +4413,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4455,7 +4441,7 @@
         <v>64</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated queue name to match naming schema
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -385,9 +385,6 @@
     <t>Minion</t>
   </si>
   <si>
-    <t>ChartStringProforma</t>
-  </si>
-  <si>
     <t>SystemError_FileServer</t>
   </si>
   <si>
@@ -518,6 +515,9 @@
   </si>
   <si>
     <t>FA_Proforma_UniFi_URL</t>
+  </si>
+  <si>
+    <t>FA_ChartStringProformaDetail</t>
   </si>
 </sst>
 </file>
@@ -878,7 +878,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -897,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -925,7 +925,7 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" t="s">
         <v>108</v>
@@ -938,8 +938,8 @@
       <c r="A3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>109</v>
+      <c r="B3" t="s">
+        <v>153</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -947,13 +947,13 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" t="s">
         <v>125</v>
-      </c>
-      <c r="C4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -962,18 +962,18 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -997,8 +997,8 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>119</v>
+      <c r="B11" s="9" t="s">
+        <v>118</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
@@ -1006,24 +1006,24 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" s="9"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -2009,11 +2009,8 @@
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" display="\\nas02.storage.uq.edu.au\CA\FBS\test\Exceptions_Screenshots"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2021,7 +2018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
@@ -2040,7 +2037,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2068,75 +2065,75 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3155,7 +3152,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -4288,7 +4285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
@@ -4312,10 +4309,10 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>142</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4323,10 +4320,10 @@
         <v>37</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -4335,25 +4332,25 @@
         <v>38</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="E3" s="8"/>
     </row>
     <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>112</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4371,7 +4368,7 @@
         <v>72</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4413,7 +4410,7 @@
         <v>45</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4441,7 +4438,7 @@
         <v>64</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Screenshot on init error, added check so screenshots are only taken if chrome errors
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -561,6 +561,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -877,8 +878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4285,7 +4286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated logo css, privatised all credential workflows and added assigns to clear passwords once the variable has been used
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="158">
   <si>
     <t>Name</t>
   </si>
@@ -518,6 +518,18 @@
   </si>
   <si>
     <t>FA_ChartStringProformaDetail</t>
+  </si>
+  <si>
+    <t>HtmlTemplate</t>
+  </si>
+  <si>
+    <t>HtmlLogo</t>
+  </si>
+  <si>
+    <t>Data\logo.png</t>
+  </si>
+  <si>
+    <t>Data\report.html</t>
   </si>
 </sst>
 </file>
@@ -879,7 +891,7 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2020,7 +2032,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3133,8 +3145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3299,12 +3311,20 @@
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
+      <c r="A20" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4286,7 +4306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ScrapeEmail.xaml Changed MHT scraping in iexplore to HTML scraping in chrome Process.xaml changed saving of email to only email body, moved sequence to ScrapeEmail.xaml so new window will be gracefully closed on exit CloseAllApplications.xaml and KillAllProcesses.xaml removed iexplore handling Renamed FA_Proforma_SSO_rpa00002 to SSO_rpa00002
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -511,9 +511,6 @@
     <t>FA_Proforma_ReportRecipients</t>
   </si>
   <si>
-    <t>FA_Proforma_SSO_rpa00002</t>
-  </si>
-  <si>
     <t>FA_Proforma_UniFi_URL</t>
   </si>
   <si>
@@ -530,6 +527,9 @@
   </si>
   <si>
     <t>Data\report.html</t>
+  </si>
+  <si>
+    <t>SSO_rpa00002</t>
   </si>
 </sst>
 </file>
@@ -952,7 +952,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -2031,8 +2031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2080,8 +2080,8 @@
       <c r="A2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B2" t="s">
-        <v>151</v>
+      <c r="B2" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
         <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2097,8 +2097,8 @@
       <c r="A5" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="B5" t="s">
-        <v>151</v>
+      <c r="B5" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2121,8 +2121,8 @@
       <c r="A9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B9" t="s">
-        <v>151</v>
+      <c r="B9" s="2" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3145,7 +3145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -3312,18 +3312,18 @@
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
EndJobReport.xaml Changed Dict(Str, Obj) to Dict(Str, Str) Config.xlsx changes to exception messages, moved environment depended settings into settings sheet with suffix report.html added rpa.ads@its.uq.edu.au InitAllSettings.xaml checks if any name ends with DEV, TEST, STAGING or PROD, will discard any that don't match the operating environment
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -169,18 +169,6 @@
     <t>Code</t>
   </si>
   <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>0.1</t>
-  </si>
-  <si>
-    <t>0.3</t>
-  </si>
-  <si>
-    <t>5.1</t>
-  </si>
-  <si>
     <t>Grants\Proposals\Maintain Staged Proposals</t>
   </si>
   <si>
@@ -190,30 +178,12 @@
     <t>System Error</t>
   </si>
   <si>
-    <t>4.2</t>
-  </si>
-  <si>
     <t>Invalid Proforma Data</t>
   </si>
   <si>
-    <t>7.1</t>
-  </si>
-  <si>
-    <t>7.2-6</t>
-  </si>
-  <si>
-    <t>8.1</t>
-  </si>
-  <si>
-    <t>8.2</t>
-  </si>
-  <si>
     <t>Accountant Not Found</t>
   </si>
   <si>
-    <t>9.1-5</t>
-  </si>
-  <si>
     <t>I couldn't match {0} to an accountant name</t>
   </si>
   <si>
@@ -238,21 +208,12 @@
     <t>RuleException_SearchRMNum</t>
   </si>
   <si>
-    <t>10.1</t>
-  </si>
-  <si>
     <t>Exchange Error</t>
   </si>
   <si>
     <t>Network Error</t>
   </si>
   <si>
-    <t>9.7-10</t>
-  </si>
-  <si>
-    <t>Invalid RM Number</t>
-  </si>
-  <si>
     <t>No Search Results</t>
   </si>
   <si>
@@ -262,12 +223,6 @@
     <t>SystemError_ProformaEntry</t>
   </si>
   <si>
-    <t>10.2-11.3</t>
-  </si>
-  <si>
-    <t>12.1-9</t>
-  </si>
-  <si>
     <t>I searched for {0} and found no results</t>
   </si>
   <si>
@@ -277,15 +232,9 @@
     <t>No Emails Found</t>
   </si>
   <si>
-    <t>14.1</t>
-  </si>
-  <si>
     <t>I couldn't create the folder at {0}</t>
   </si>
   <si>
-    <t>14.2</t>
-  </si>
-  <si>
     <t>SystemError_CreateFolder</t>
   </si>
   <si>
@@ -298,9 +247,6 @@
     <t>UniFiPath_MaintainStagedProposals</t>
   </si>
   <si>
-    <t>SystemError_CheckExchange</t>
-  </si>
-  <si>
     <t>UniFi Login Error</t>
   </si>
   <si>
@@ -319,9 +265,6 @@
     <t>SystemError_UnhandledUniFi</t>
   </si>
   <si>
-    <t>9.1-12.9</t>
-  </si>
-  <si>
     <t>UniFi Unknown Error</t>
   </si>
   <si>
@@ -337,9 +280,6 @@
     <t>SystemError_UnhandledExchange</t>
   </si>
   <si>
-    <t>7.1-6</t>
-  </si>
-  <si>
     <t>Unknown Scrape Error</t>
   </si>
   <si>
@@ -364,9 +304,6 @@
     <t>Problems with {0}'s mail: {1} at: {2}</t>
   </si>
   <si>
-    <t>Problems checking {0} as {1}: {2} at {3}</t>
-  </si>
-  <si>
     <t>Login issue as {0} to UniFi at {1}: {2} at {3}</t>
   </si>
   <si>
@@ -388,9 +325,6 @@
     <t>SystemError_FileServer</t>
   </si>
   <si>
-    <t>0.2</t>
-  </si>
-  <si>
     <t>File Server Access</t>
   </si>
   <si>
@@ -439,21 +373,12 @@
     <t>Sheet1</t>
   </si>
   <si>
-    <t>UniFi_URL</t>
-  </si>
-  <si>
-    <t>NetworkShare_DownloadFolder</t>
-  </si>
-  <si>
     <t>Credentials_UniFi</t>
   </si>
   <si>
     <t>Credentials_FileServing</t>
   </si>
   <si>
-    <t>Accountant_LookupWorkbook</t>
-  </si>
-  <si>
     <t>Credentials_Exchange</t>
   </si>
   <si>
@@ -466,12 +391,6 @@
     <t>JobReport_Recipients</t>
   </si>
   <si>
-    <t>SystemError_NotificationEmail</t>
-  </si>
-  <si>
-    <t>SystemError_Recipients</t>
-  </si>
-  <si>
     <t>ExchangeInbox</t>
   </si>
   <si>
@@ -490,30 +409,15 @@
     <t>Description (Assets will always overwrite other config)</t>
   </si>
   <si>
-    <t>Exchange_Mailbox</t>
-  </si>
-  <si>
     <t>\New</t>
   </si>
   <si>
     <t>\Error</t>
   </si>
   <si>
-    <t>FA_Proforma_Exchange_RootFolder</t>
-  </si>
-  <si>
-    <t>FA_Proforma_FileShare_AccountantLookup</t>
-  </si>
-  <si>
-    <t>FA_Proforma_FileShare_SaveFolder</t>
-  </si>
-  <si>
     <t>FA_Proforma_ReportRecipients</t>
   </si>
   <si>
-    <t>FA_Proforma_UniFi_URL</t>
-  </si>
-  <si>
     <t>FA_ChartStringProformaDetail</t>
   </si>
   <si>
@@ -530,13 +434,136 @@
   </si>
   <si>
     <t>SSO_rpa00002</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Inbox\Proforma - Dev</t>
+  </si>
+  <si>
+    <t>Exchange_Mailbox-DEV</t>
+  </si>
+  <si>
+    <t>Exchange_Mailbox-TEST</t>
+  </si>
+  <si>
+    <t>Exchange_Mailbox-STAGING</t>
+  </si>
+  <si>
+    <t>Exchange_Mailbox-PROD</t>
+  </si>
+  <si>
+    <t>contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma\Staging</t>
+  </si>
+  <si>
+    <t>contractandgrants@uq.edu.au\Inbox\Minion - GRL Proforma</t>
+  </si>
+  <si>
+    <t>Inbox\Proforma - Testing</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\FBS\Contract and Grants Accounting\General\GRLS\Minion-Staging\Accountant Lookup.xlsx</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\FBS\Contract and Grants Accounting\General\GRLS\Accountant Lookup.xlsx</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\FBS\Contract and Grants Accounting\General\GRLS\Minion-Staging\{0}\</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\FBS\Contract and Grants Accounting\General\GRLS\No project GRLS\{0}\</t>
+  </si>
+  <si>
+    <t>NetworkShare_DownloadFolder-DEV</t>
+  </si>
+  <si>
+    <t>NetworkShare_DownloadFolder-TEST</t>
+  </si>
+  <si>
+    <t>NetworkShare_DownloadFolder-STAGING</t>
+  </si>
+  <si>
+    <t>NetworkShare_DownloadFolder-PROD</t>
+  </si>
+  <si>
+    <t>Accountant_LookupWorkbook-DEV</t>
+  </si>
+  <si>
+    <t>Accountant_LookupWorkbook-TEST</t>
+  </si>
+  <si>
+    <t>Accountant_LookupWorkbook-STAGING</t>
+  </si>
+  <si>
+    <t>Accountant_LookupWorkbook-PROD</t>
+  </si>
+  <si>
+    <t>UniFi_URL-DEV</t>
+  </si>
+  <si>
+    <t>UniFi_URL-TEST</t>
+  </si>
+  <si>
+    <t>UniFi_URL-STAGING</t>
+  </si>
+  <si>
+    <t>UniFi_URL-PROD</t>
+  </si>
+  <si>
+    <t>https://fs92fnta.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
+  </si>
+  <si>
+    <t>https://fs92prep.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
+  </si>
+  <si>
+    <t>https://www.unifi.uq.edu.au/psp/ps/?cmd=login</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\DEV\FA_ChartStringProformaDetail\{0}\</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\TEST\FA_ChartStringProformaDetail\{0}\</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\DEV\FA_ChartStringProformaDetail\Accountant Lookup.xlsx</t>
+  </si>
+  <si>
+    <t>\\nas02.storage.uq.edu.au\CA\ITS\Academic Services\RPA\TEST\FA_ChartStringProformaDetail\Accountant Lookup.xlsx</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Invalid Email Format</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -575,6 +602,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -593,10 +634,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -608,8 +650,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -891,13 +937,13 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="112.28515625" customWidth="1"/>
     <col min="3" max="3" width="118.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -910,7 +956,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -938,10 +984,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
@@ -952,7 +998,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -960,99 +1006,176 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="9"/>
-    </row>
-    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+    </row>
+    <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="10"/>
+    </row>
+    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="10"/>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" s="10"/>
+    </row>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-    </row>
-    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="C9" s="10"/>
+    </row>
+    <row r="10" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>139</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="C11" t="s">
-        <v>10</v>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>140</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
+        <v>141</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>142</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="B13" s="9" t="s">
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B14" s="9"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="B17" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="9"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="9"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="9"/>
     </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="9"/>
+    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="9"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="C31" s="9"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="9"/>
     </row>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2031,8 +2154,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2050,7 +2173,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>143</v>
+        <v>116</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2078,106 +2201,61 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="B3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>106</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>131</v>
-      </c>
-      <c r="B7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B10" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="B11" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B12" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="9"/>
-    </row>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="9"/>
-    </row>
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="9"/>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3146,7 +3224,7 @@
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3165,7 +3243,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3193,148 +3271,204 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>5000</v>
+        <v>9</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>30000</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4">
-        <v>120000</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
+      <c r="A4" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>1000</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
+      <c r="A6" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7">
-        <v>15000</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
-        <v>60000</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
+      <c r="A7" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>5000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>30000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
+        <v>120000</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23">
+        <v>1000</v>
+      </c>
+      <c r="C23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B24">
+        <v>15000</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>60000</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>17</v>
       </c>
-      <c r="B10">
+      <c r="B27">
         <v>0.6</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C27" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="28" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>19</v>
       </c>
-      <c r="B11">
+      <c r="B28">
         <v>0.8</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C28" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="29" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>21</v>
       </c>
-      <c r="B12">
+      <c r="B29">
         <v>0.9</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>104</v>
-      </c>
-      <c r="B15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4304,10 +4438,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4330,342 +4464,324 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>141</v>
+        <v>114</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>142</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>37</v>
+        <v>126</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
-        <v>38</v>
+        <v>126</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>113</v>
-      </c>
-    </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>40</v>
+        <v>88</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>126</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>121</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>49</v>
+        <v>44</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>155</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>60</v>
+        <v>45</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>160</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>119</v>
+        <v>63</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>68</v>
+        <v>161</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>89</v>
+        <v>57</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>163</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>64</v>
+        <v>162</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>120</v>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>48</v>
+        <v>164</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>100</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>73</v>
+        <v>71</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>164</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>74</v>
+        <v>53</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>44</v>
+        <v>59</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>101</v>
+        <v>51</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>44</v>
+        <v>73</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>163</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>93</v>
+        <v>46</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>160</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>166</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>103</v>
+        <v>65</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>63</v>
+        <v>165</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>78</v>
-      </c>
+      <c r="D22" s="5"/>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D24" s="5"/>
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="C26" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" t="s">
-        <v>24</v>
-      </c>
-      <c r="D28" t="s">
-        <v>25</v>
+        <v>76</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C29" t="s">
-        <v>29</v>
-      </c>
-      <c r="D29" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>97</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="2" t="s">
-        <v>99</v>
+        <v>77</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating exception messages to finalise reporting format and content. Still work in progress
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="164">
   <si>
     <t>Name</t>
   </si>
@@ -178,9 +178,6 @@
     <t>System Error</t>
   </si>
   <si>
-    <t>Invalid Proforma Data</t>
-  </si>
-  <si>
     <t>Accountant Not Found</t>
   </si>
   <si>
@@ -214,12 +211,6 @@
     <t>Network Error</t>
   </si>
   <si>
-    <t>No Search Results</t>
-  </si>
-  <si>
-    <t>No Updated Entries</t>
-  </si>
-  <si>
     <t>SystemError_ProformaEntry</t>
   </si>
   <si>
@@ -229,12 +220,6 @@
     <t>RuleException_NoEmails</t>
   </si>
   <si>
-    <t>No Emails Found</t>
-  </si>
-  <si>
-    <t>I couldn't create the folder at {0}</t>
-  </si>
-  <si>
     <t>SystemError_CreateFolder</t>
   </si>
   <si>
@@ -247,15 +232,6 @@
     <t>UniFiPath_MaintainStagedProposals</t>
   </si>
   <si>
-    <t>UniFi Login Error</t>
-  </si>
-  <si>
-    <t>UniFi Navigation Error</t>
-  </si>
-  <si>
-    <t>UniFi Updating Error</t>
-  </si>
-  <si>
     <t>RuleException_SearchAccountant</t>
   </si>
   <si>
@@ -265,12 +241,6 @@
     <t>SystemError_UnhandledUniFi</t>
   </si>
   <si>
-    <t>UniFi Unknown Error</t>
-  </si>
-  <si>
-    <t>I wasn't able to update {0} as the rows were: {1}</t>
-  </si>
-  <si>
     <t>RuleException_UpdateProforma</t>
   </si>
   <si>
@@ -280,9 +250,6 @@
     <t>SystemError_UnhandledExchange</t>
   </si>
   <si>
-    <t>Unknown Scrape Error</t>
-  </si>
-  <si>
     <t>I couldn't scrape proforma data from the email {0}</t>
   </si>
   <si>
@@ -298,15 +265,6 @@
     <t>Row {0} updated, {1}</t>
   </si>
   <si>
-    <t>Problems loading {0} for Acc lookup: {1} at: {2}</t>
-  </si>
-  <si>
-    <t>Problems with {0}'s mail: {1} at: {2}</t>
-  </si>
-  <si>
-    <t>Login issue as {0} to UniFi at {1}: {2} at {3}</t>
-  </si>
-  <si>
     <t>ExchangeExitErrors</t>
   </si>
   <si>
@@ -325,9 +283,6 @@
     <t>SystemError_FileServer</t>
   </si>
   <si>
-    <t>File Server Access</t>
-  </si>
-  <si>
     <t>Mode Asset Missing</t>
   </si>
   <si>
@@ -544,9 +499,6 @@
     <t>5</t>
   </si>
   <si>
-    <t>Invalid Email Format</t>
-  </si>
-  <si>
     <t>7</t>
   </si>
   <si>
@@ -557,6 +509,45 @@
   </si>
   <si>
     <t>12</t>
+  </si>
+  <si>
+    <t>UniFi Error</t>
+  </si>
+  <si>
+    <t>I wasn't able to update {0} as no rows were updated: {1}</t>
+  </si>
+  <si>
+    <t>Email Error</t>
+  </si>
+  <si>
+    <t>I couldn't login as {0} to UniFi at {1}: {2} at {3}</t>
+  </si>
+  <si>
+    <t>I couldn't access {0} for Acc lookup: {1} at: {2}</t>
+  </si>
+  <si>
+    <t>I couldn't access my email as {0}: {1} at: {2}</t>
+  </si>
+  <si>
+    <t>Report_EmailOnSuccess</t>
+  </si>
+  <si>
+    <t>EmailOnSuccess</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_PORT</t>
+  </si>
+  <si>
+    <t>UQ_SMTP_SERVER</t>
+  </si>
+  <si>
+    <t>Report_SmtpPort</t>
+  </si>
+  <si>
+    <t>Report_SmtpServer</t>
+  </si>
+  <si>
+    <t>I couldn't create the folder {0} at {1}</t>
   </si>
 </sst>
 </file>
@@ -956,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -984,10 +975,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
         <v>35</v>
@@ -998,7 +989,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -1006,13 +997,13 @@
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1022,37 +1013,37 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C9" s="10"/>
     </row>
@@ -1063,66 +1054,66 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B15" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>129</v>
+      </c>
+      <c r="B16" s="9" t="s">
         <v>144</v>
-      </c>
-      <c r="B16" s="9" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1131,36 +1122,36 @@
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2155,7 +2146,7 @@
   <dimension ref="A1:Z989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2173,7 +2164,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2201,38 +2192,60 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+    </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3223,8 +3236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3243,7 +3256,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3274,7 +3287,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -3283,78 +3296,78 @@
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>37</v>
@@ -4440,8 +4453,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:D29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4464,255 +4477,255 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="E3" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>81</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>155</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>63</v>
+        <v>151</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>82</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>40</v>
+        <v>153</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>53</v>
+        <v>151</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>70</v>
+        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>165</v>
+        <v>63</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>58</v>
+        <v>153</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>163</v>
+        <v>45</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>145</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>74</v>
+        <v>151</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>64</v>
+        <v>151</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>166</v>
+      <c r="B20" s="6" t="s">
+        <v>149</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>50</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>69</v>
+        <v>151</v>
       </c>
       <c r="D22" s="5"/>
     </row>
@@ -4721,7 +4734,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C24" t="s">
         <v>39</v>
@@ -4735,7 +4748,7 @@
         <v>31</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="C25" t="s">
         <v>39</v>
@@ -4768,20 +4781,20 @@
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="2" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="2" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated exception messages to match confluence pages
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -2145,8 +2145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3236,7 +3236,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z994"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -4454,7 +4454,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated config to use FS92FNTA instead of FS92PREP for UniFi in STAGING
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -467,9 +467,6 @@
   </si>
   <si>
     <t>https://fs92fnta.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
-  </si>
-  <si>
-    <t>https://fs92prep.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
   </si>
   <si>
     <t>https://www.unifi.uq.edu.au/psp/ps/?cmd=login</t>
@@ -927,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1057,7 +1054,7 @@
         <v>124</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1065,7 +1062,7 @@
         <v>125</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
@@ -1089,7 +1086,7 @@
         <v>128</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
@@ -1097,7 +1094,7 @@
         <v>129</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1143,7 +1140,7 @@
         <v>134</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1151,7 +1148,7 @@
         <v>135</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2145,8 +2142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2224,26 +2221,26 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>156</v>
+      </c>
+      <c r="B6" t="s">
         <v>157</v>
-      </c>
-      <c r="B6" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4512,13 +4509,13 @@
         <v>42</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4540,13 +4537,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4554,13 +4551,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4568,7 +4565,7 @@
         <v>53</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>49</v>
@@ -4582,10 +4579,10 @@
         <v>47</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>83</v>
@@ -4596,10 +4593,10 @@
         <v>46</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>82</v>
@@ -4610,7 +4607,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>40</v>
@@ -4624,10 +4621,10 @@
         <v>48</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>52</v>
@@ -4638,13 +4635,13 @@
         <v>61</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4652,10 +4649,10 @@
         <v>63</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>64</v>
@@ -4666,10 +4663,10 @@
         <v>45</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>59</v>
@@ -4680,10 +4677,10 @@
         <v>51</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>62</v>
@@ -4694,13 +4691,13 @@
         <v>54</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4708,7 +4705,7 @@
         <v>55</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>50</v>
@@ -4722,10 +4719,10 @@
         <v>60</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D22" s="5"/>
     </row>

</xml_diff>

<commit_message>
Config.xlsx - Added asset SendEmailOn EndJobReport.xaml - Uses SendEmailOn to determine what level reporting the bot is undertaking. Adds the environment or machine name to the robot name if running in non prod environments.
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="165">
   <si>
     <t>Name</t>
   </si>
@@ -526,12 +526,6 @@
     <t>I couldn't access my email as {0}: {1} at: {2}</t>
   </si>
   <si>
-    <t>Report_EmailOnSuccess</t>
-  </si>
-  <si>
-    <t>EmailOnSuccess</t>
-  </si>
-  <si>
     <t>UQ_SMTP_PORT</t>
   </si>
   <si>
@@ -545,6 +539,18 @@
   </si>
   <si>
     <t>I couldn't create the folder {0} at {1}</t>
+  </si>
+  <si>
+    <t>Report_SendEmailOn</t>
+  </si>
+  <si>
+    <t>FA_Proforma_SendEmailOn</t>
+  </si>
+  <si>
+    <t>List of names to send the report email to, leave as ';' if no recipients</t>
+  </si>
+  <si>
+    <t>When to send a report email, 'ALWAYS' for after any job, 'SUCCESS' for only if transactions have been processed, 'ERROR' for only if transactions have failed or 'NEVER' for reporting to be silent.</t>
   </si>
 </sst>
 </file>
@@ -924,7 +930,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -2142,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2218,29 +2224,35 @@
       <c r="B5" t="s">
         <v>104</v>
       </c>
+      <c r="C5" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="B6" t="s">
-        <v>157</v>
+        <v>162</v>
+      </c>
+      <c r="C6" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B8" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4697,7 +4709,7 @@
         <v>50</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Set staging environment to use FS92PREP instead of FS92FNTA.
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71916D32-CC68-45F2-BD64-0B7DB991BA52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8055" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,12 +23,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Samuel Janetzki</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="166">
   <si>
     <t>Name</t>
   </si>
@@ -551,12 +552,15 @@
   </si>
   <si>
     <t>When to send a report email, 'ALWAYS' for after any job, 'SUCCESS' for only if transactions have been processed, 'ERROR' for only if transactions have failed or 'NEVER' for reporting to be silent.</t>
+  </si>
+  <si>
+    <t>https://fs92prep.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -927,11 +931,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1146,7 +1150,7 @@
         <v>134</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>136</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2145,11 +2149,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z989"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3242,7 +3246,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z994"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4459,7 +4463,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
ITSADSSD-20635: Removes duplicate spaces when scraping short description. Fixed typo in log message in config.
</commit_message>
<xml_diff>
--- a/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
+++ b/Processes/FA_ChartStringProformaDetail/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spamish\Documents\UiPath\RpaUiPathProcess\Processes\FA_ChartStringProformaDetail\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71916D32-CC68-45F2-BD64-0B7DB991BA52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0CE19A-EC75-4223-87D7-6F152649C63D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -149,9 +149,6 @@
     <t>Transaction Successful.</t>
   </si>
   <si>
-    <t>Static part of logging message. Processed Transaction succesful</t>
-  </si>
-  <si>
     <t>LogMessage_ApplicationException</t>
   </si>
   <si>
@@ -555,6 +552,9 @@
   </si>
   <si>
     <t>https://fs92prep.dev.unifi.uq.edu.au/psp/ps/?cmd=login</t>
+  </si>
+  <si>
+    <t>Static part of logging message. Processed Transaction successful</t>
   </si>
 </sst>
 </file>
@@ -934,7 +934,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
@@ -954,7 +954,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -982,35 +982,35 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C3" t="s">
         <v>33</v>
-      </c>
-      <c r="B3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" t="s">
         <v>87</v>
-      </c>
-      <c r="C4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1020,37 +1020,37 @@
     </row>
     <row r="6" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C7" s="10"/>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C8" s="10"/>
     </row>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C9" s="10"/>
     </row>
@@ -1061,66 +1061,66 @@
     </row>
     <row r="11" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1129,36 +1129,36 @@
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="11"/>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2171,7 +2171,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2199,64 +2199,64 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6" t="s">
         <v>161</v>
       </c>
-      <c r="B6" t="s">
-        <v>162</v>
-      </c>
       <c r="C6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3269,7 +3269,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -3300,7 +3300,7 @@
         <v>9</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" t="s">
         <v>10</v>
@@ -3309,84 +3309,84 @@
     <row r="3" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="9"/>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
         <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4466,8 +4466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4484,261 +4484,261 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>99</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="E3" s="8"/>
     </row>
     <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="D19" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D22" s="5"/>
     </row>
@@ -4747,10 +4747,10 @@
         <v>26</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D24" t="s">
         <v>27</v>
@@ -4758,16 +4758,16 @@
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" t="s">
         <v>31</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" t="s">
-        <v>39</v>
-      </c>
-      <c r="D25" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4789,25 +4789,25 @@
         <v>29</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>165</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>